<commit_message>
CV pantalla de compras reportes, integración de pagos
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-Compras.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-Compras.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CAF766-DFED-9F46-B7FE-6C34BAAE84AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CECFB4-D1FD-2949-AE7C-46ED267E055C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="6880" windowWidth="32080" windowHeight="17380" xr2:uid="{306FDEFB-6B54-2B40-874B-FA2C57B165FD}"/>
+    <workbookView xWindow="1040" yWindow="3140" windowWidth="46420" windowHeight="21220" xr2:uid="{306FDEFB-6B54-2B40-874B-FA2C57B165FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ESTABLECIMIENTO :</t>
   </si>
@@ -42,9 +42,6 @@
     <t>FECHA</t>
   </si>
   <si>
-    <t># FACT</t>
-  </si>
-  <si>
     <t>RUC / CI</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>TIP COMP</t>
   </si>
   <si>
-    <t># AUTORIZACION</t>
-  </si>
-  <si>
     <t>ESTADO</t>
   </si>
   <si>
@@ -72,52 +66,22 @@
     <t>RETENCION</t>
   </si>
   <si>
-    <t>TIPO PAGO</t>
-  </si>
-  <si>
-    <t>FACTURA</t>
-  </si>
-  <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>DESCRIPCION</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>P. UNITARIO</t>
-  </si>
-  <si>
-    <t>P. TOTAL</t>
-  </si>
-  <si>
-    <t>% IVA</t>
-  </si>
-  <si>
-    <t>DETALLE</t>
-  </si>
-  <si>
-    <t>TIP PAGO</t>
-  </si>
-  <si>
-    <t>DOCUMENTO</t>
-  </si>
-  <si>
-    <t>BANCO</t>
-  </si>
-  <si>
-    <t>VALOR</t>
-  </si>
-  <si>
     <t>LISTADO DE COMPRAS</t>
   </si>
   <si>
-    <t>TOTAL FAC</t>
-  </si>
-  <si>
-    <t>VAL PAGAR</t>
+    <t>NUM COM</t>
+  </si>
+  <si>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>A PAGAR</t>
+  </si>
+  <si>
+    <t>PAGO</t>
   </si>
 </sst>
 </file>
@@ -196,19 +160,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,27 +487,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A527F97D-E6F1-DE46-8C92-B6BC6FE0A79B}">
-  <dimension ref="A2:AA10"/>
+  <dimension ref="A2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -558,201 +519,106 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T10" s="4" t="s">
+      <c r="M9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="V10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="A2:AA2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="A9:N9"/>
-    <mergeCell ref="T9:AA9"/>
+  <mergeCells count="5">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CV Compras, aumentar si es un gasto
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-Compras.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-Compras.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CECFB4-D1FD-2949-AE7C-46ED267E055C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601F15CF-7F43-2441-A9DA-E9C7EC419682}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="3140" windowWidth="46420" windowHeight="21220" xr2:uid="{306FDEFB-6B54-2B40-874B-FA2C57B165FD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ESTABLECIMIENTO :</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>PAGO</t>
+  </si>
+  <si>
+    <t>GASTO</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,10 +170,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A527F97D-E6F1-DE46-8C92-B6BC6FE0A79B}">
-  <dimension ref="A2:N9"/>
+  <dimension ref="A2:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,29 +504,30 @@
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -529,8 +536,9 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -539,8 +547,9 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -549,8 +558,9 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -559,16 +569,18 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -587,28 +599,31 @@
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -618,7 +633,7 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>